<commit_message>
Updated database modeling and dictionnary with all new stuff
</commit_message>
<xml_diff>
--- a/docs-bdd/CRM - Dictionnaire base de données.xlsx
+++ b/docs-bdd/CRM - Dictionnaire base de données.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$A$1:$E$26</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$A$1:$E$30</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
   <si>
     <t>Entité</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Contraintes</t>
-  </si>
-  <si>
-    <t>LES ENTITÉS</t>
   </si>
   <si>
     <t>brand</t>
@@ -57,9 +54,6 @@
     <t>VARCHAR(7)</t>
   </si>
   <si>
-    <t>campaign</t>
-  </si>
-  <si>
     <t>budgets</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>DECIMAL(15,2)</t>
   </si>
   <si>
-    <t>operation</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -84,16 +75,13 @@
     <t>INT</t>
   </si>
   <si>
-    <t>partner</t>
+    <t>campaign</t>
   </si>
   <si>
     <t>budget</t>
   </si>
   <si>
     <t>Le budget total que le client investi dans une campagne</t>
-  </si>
-  <si>
-    <t>target</t>
   </si>
   <si>
     <t>campaign_name</t>
@@ -111,16 +99,10 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>media</t>
-  </si>
-  <si>
     <t>date_start</t>
   </si>
   <si>
     <t>La date de départ d'une campagne de communication</t>
-  </si>
-  <si>
-    <t>users</t>
   </si>
   <si>
     <t>id_user_TDC</t>
@@ -138,19 +120,40 @@
     <t>Le nom d'une entreprise</t>
   </si>
   <si>
+    <t>logo_url</t>
+  </si>
+  <si>
+    <t>URL du logo téléchargé à la création du client</t>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>unique_brand</t>
+  </si>
+  <si>
+    <t>Si un client à une ou plusieurs marques</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
     <t>media_name</t>
   </si>
   <si>
     <t>Le nom du media de communication</t>
   </si>
   <si>
+    <t>operation</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
     <t>Description libre de l'opération</t>
-  </si>
-  <si>
-    <t>VARCHAR(255)</t>
   </si>
   <si>
     <t>operation_date</t>
@@ -165,10 +168,22 @@
     <t>Prix d'une opération HT</t>
   </si>
   <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>partner_colour</t>
+  </si>
+  <si>
+    <t>La couleur de la légende d'un partenaire</t>
+  </si>
+  <si>
     <t>partner_name</t>
   </si>
   <si>
     <t>Le nom du partenaire d'une opération</t>
+  </si>
+  <si>
+    <t>target</t>
   </si>
   <si>
     <t>target_com</t>
@@ -186,13 +201,13 @@
     <t>Couleur de légende des objectifs de campagne de comm</t>
   </si>
   <si>
+    <t>users</t>
+  </si>
+  <si>
     <t>boss</t>
   </si>
   <si>
     <t>Si l'utilisateur est patron de l'entreprise ou non</t>
-  </si>
-  <si>
-    <t>BOOLEAN</t>
   </si>
   <si>
     <t>NOT NULL; DEFAULT 0;</t>
@@ -211,6 +226,12 @@
   </si>
   <si>
     <t>Email de l'utilisateur</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>Si le compte utilisateur est autorisé ou non</t>
   </si>
   <si>
     <t>firstname</t>
@@ -546,9 +567,7 @@
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="H1" s="3"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -570,24 +589,22 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="2"/>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="H2" s="4"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -609,24 +626,22 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="H3" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="H3" s="4"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -648,24 +663,22 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="H4" s="4"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -687,24 +700,22 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="H5" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="H5" s="4"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -726,24 +737,22 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="H6" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="H6" s="4"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -765,24 +774,22 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F7" s="2"/>
-      <c r="H7" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="H7" s="4"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -804,24 +811,22 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="H8" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -843,24 +848,22 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="H9" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="H9" s="4"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -882,19 +885,19 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="4"/>
@@ -919,19 +922,19 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2"/>
       <c r="I11" s="2"/>
@@ -958,16 +961,16 @@
         <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="2"/>
@@ -991,22 +994,21 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1028,23 +1030,21 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1066,23 +1066,22 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1104,19 +1103,19 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1142,19 +1141,19 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1180,19 +1179,19 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1218,19 +1217,19 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1256,19 +1255,19 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1294,19 +1293,19 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1332,19 +1331,19 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1370,19 +1369,19 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1408,19 +1407,19 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1446,19 +1445,19 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1484,19 +1483,19 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1521,11 +1520,21 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="A27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1549,11 +1558,21 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1577,11 +1596,21 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="A29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1605,11 +1634,21 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="A30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -28848,11 +28887,95 @@
       <c r="Y1002" s="2"/>
       <c r="Z1002" s="2"/>
     </row>
+    <row r="1003">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="2"/>
+      <c r="H1004" s="2"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="2"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="2"/>
+      <c r="M1004" s="2"/>
+      <c r="N1004" s="2"/>
+      <c r="O1004" s="2"/>
+      <c r="P1004" s="2"/>
+      <c r="Q1004" s="2"/>
+      <c r="R1004" s="2"/>
+      <c r="S1004" s="2"/>
+      <c r="T1004" s="2"/>
+      <c r="U1004" s="2"/>
+      <c r="V1004" s="2"/>
+      <c r="W1004" s="2"/>
+      <c r="X1004" s="2"/>
+      <c r="Y1004" s="2"/>
+      <c r="Z1004" s="2"/>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="2"/>
+      <c r="B1005" s="2"/>
+      <c r="C1005" s="2"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="2"/>
+      <c r="F1005" s="2"/>
+      <c r="G1005" s="2"/>
+      <c r="H1005" s="2"/>
+      <c r="I1005" s="2"/>
+      <c r="J1005" s="2"/>
+      <c r="K1005" s="2"/>
+      <c r="L1005" s="2"/>
+      <c r="M1005" s="2"/>
+      <c r="N1005" s="2"/>
+      <c r="O1005" s="2"/>
+      <c r="P1005" s="2"/>
+      <c r="Q1005" s="2"/>
+      <c r="R1005" s="2"/>
+      <c r="S1005" s="2"/>
+      <c r="T1005" s="2"/>
+      <c r="U1005" s="2"/>
+      <c r="V1005" s="2"/>
+      <c r="W1005" s="2"/>
+      <c r="X1005" s="2"/>
+      <c r="Y1005" s="2"/>
+      <c r="Z1005" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$26">
-    <sortState ref="A1:E26">
-      <sortCondition ref="A1:A26"/>
-      <sortCondition ref="B1:B26"/>
+  <autoFilter ref="$A$1:$E$30">
+    <sortState ref="A1:E30">
+      <sortCondition ref="A1:A30"/>
+      <sortCondition ref="B1:B30"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>

</xml_diff>